<commit_message>
bug fixes for imports
</commit_message>
<xml_diff>
--- a/server/public/templates/residents-template.xlsx
+++ b/server/public/templates/residents-template.xlsx
@@ -4,7 +4,6 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nama Lengkap</t>
   </si>
@@ -53,65 +52,17 @@
     <t>Kewarganegaraan</t>
   </si>
   <si>
-    <t>Alamat</t>
+    <t>Status NIK</t>
   </si>
   <si>
-    <t>Domisili</t>
-  </si>
-  <si>
-    <t>BUDI HARDJO SUPRAPTO</t>
-  </si>
-  <si>
-    <t>3175072501098422</t>
-  </si>
-  <si>
-    <t>3175072207630007</t>
-  </si>
-  <si>
-    <t>ELLI ROSITA SUHARDINI</t>
-  </si>
-  <si>
-    <t>3175075608620002</t>
-  </si>
-  <si>
-    <t>CITRA AZKA RADITYA T.</t>
-  </si>
-  <si>
-    <t>3175075812930001</t>
-  </si>
-  <si>
-    <t>SIDIK PURNAMA HIDAYAT</t>
-  </si>
-  <si>
-    <t>317507301190006</t>
-  </si>
-  <si>
-    <t>3211181210900004</t>
-  </si>
-  <si>
-    <t>DITA INDAH PERMATA SARI</t>
-  </si>
-  <si>
-    <t>317507420890001</t>
-  </si>
-  <si>
-    <t>FARZAN SALIM BARACK</t>
-  </si>
-  <si>
-    <t>3175070812200008</t>
-  </si>
-  <si>
-    <t>07</t>
+    <t>Alasan tidak aktif</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/MM/yyyy"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -130,17 +81,8 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,14 +95,8 @@
         <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="2">
     <border/>
     <border>
       <left style="thin">
@@ -176,123 +112,11 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -304,53 +128,12 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="3" fontId="3" numFmtId="49" xfId="0" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="3" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="6" fillId="3" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="7" fillId="3" fontId="4" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="11" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="12" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="13" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -361,10 +144,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -582,6 +361,7 @@
     <col customWidth="1" min="11" max="11" width="20.0"/>
     <col customWidth="1" min="12" max="12" width="17.63"/>
     <col customWidth="1" min="13" max="13" width="18.25"/>
+    <col customWidth="1" min="15" max="15" width="17.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -639,14 +419,14 @@
       <c r="E2" s="4"/>
       <c r="F2" s="6"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="4"/>
@@ -656,14 +436,14 @@
       <c r="E3" s="4"/>
       <c r="F3" s="6"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="4"/>
@@ -673,14 +453,14 @@
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="4"/>
@@ -689,15 +469,15 @@
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="4"/>
@@ -707,14 +487,14 @@
       <c r="E6" s="4"/>
       <c r="F6" s="6"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="4"/>
@@ -9080,231 +8860,30 @@
       <c r="N498" s="4"/>
       <c r="O498" s="4"/>
     </row>
-    <row r="499">
-      <c r="A499" s="4"/>
-      <c r="B499" s="4"/>
-      <c r="C499" s="4"/>
-      <c r="D499" s="4"/>
-      <c r="E499" s="4"/>
-      <c r="F499" s="4"/>
-      <c r="G499" s="4"/>
-      <c r="H499" s="4"/>
-      <c r="I499" s="4"/>
-      <c r="J499" s="4"/>
-      <c r="K499" s="4"/>
-      <c r="L499" s="4"/>
-      <c r="M499" s="4"/>
-      <c r="N499" s="4"/>
-      <c r="O499" s="4"/>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="19.25"/>
-    <col customWidth="1" min="2" max="3" width="15.88"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="15">
-        <v>31.0</v>
-      </c>
-      <c r="B8" s="16">
-        <v>75.0</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="17">
-        <v>2.501098422E9</v>
-      </c>
-      <c r="E8" s="8" t="str">
-        <f t="shared" ref="E8:E14" si="1">CONCATENATE(A8,B8,C8,D8)</f>
-        <v>3175072501098422</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="15">
-        <v>31.0</v>
-      </c>
-      <c r="B9" s="16">
-        <v>75.0</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="17">
-        <v>2.501098422E9</v>
-      </c>
-      <c r="E9" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>3175072501098422</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="18">
-        <v>31.0</v>
-      </c>
-      <c r="B10" s="19">
-        <v>75.0</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="20">
-        <v>2.501098422E9</v>
-      </c>
-      <c r="E10" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>3175072501098422</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="21"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="15">
-        <v>31.0</v>
-      </c>
-      <c r="B12" s="16">
-        <v>75.0</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="17">
-        <v>3.01190006E8</v>
-      </c>
-      <c r="E12" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>317507301190006</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="15">
-        <v>31.0</v>
-      </c>
-      <c r="B13" s="16">
-        <v>75.0</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="17">
-        <v>3.01190006E8</v>
-      </c>
-      <c r="E13" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>317507301190006</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="24">
-        <v>31.0</v>
-      </c>
-      <c r="B14" s="25">
-        <v>75.0</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="26">
-        <v>3.01190006E8</v>
-      </c>
-      <c r="E14" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>317507301190006</v>
-      </c>
-    </row>
-  </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D498">
+      <formula1>"Laki - Laki,Perempuan"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J498">
+      <formula1>"Kepala Keluarga,Istri,Anak"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G498">
+      <formula1>"A,B,O"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I498">
+      <formula1>"Belum Menikah,Menikah,Janda,Duda"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L2:L498">
+      <formula1>"PNS,Pegawai Swasta,TNI,POLRI,Guru,Petani,Pedagang,Wiraswasta,Pelajar,Mahasiswa,Buruh,Pengangguran,Pensiunan,Lainnya"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N2:N498">
+      <formula1>"aktif,tidak aktif - meninggal,tidak aktif - pindah,tidak aktif - lainnya"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H498">
+      <formula1>"Islam,Protestan,Katolik,Hindu,Buddha,Konghuchu"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>